<commit_message>
adding goals info back to the df and datetime FE
</commit_message>
<xml_diff>
--- a/data_protocol/teamstats_datatype.xlsx
+++ b/data_protocol/teamstats_datatype.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B44"/>
+  <dimension ref="A1:B48"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -513,19 +513,19 @@
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>home_xGoals</t>
+          <t>homeGoals</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="1" t="inlineStr">
         <is>
-          <t>home_shots</t>
+          <t>awayGoals</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
@@ -537,7 +537,7 @@
     <row r="10">
       <c r="A10" s="1" t="inlineStr">
         <is>
-          <t>home_shotsOnTarget</t>
+          <t>homeGoalsHalfTime</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
@@ -549,7 +549,7 @@
     <row r="11">
       <c r="A11" s="1" t="inlineStr">
         <is>
-          <t>home_deep</t>
+          <t>awayGoalsHalfTime</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
@@ -561,7 +561,7 @@
     <row r="12">
       <c r="A12" s="1" t="inlineStr">
         <is>
-          <t>home_ppda</t>
+          <t>home_xGoals</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
@@ -573,7 +573,7 @@
     <row r="13">
       <c r="A13" s="1" t="inlineStr">
         <is>
-          <t>home_fouls</t>
+          <t>home_shots</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
@@ -585,7 +585,7 @@
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>home_corners</t>
+          <t>home_shotsOnTarget</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
@@ -597,31 +597,31 @@
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>home_yellowCards</t>
+          <t>home_deep</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="1" t="inlineStr">
         <is>
-          <t>home_redCards</t>
+          <t>home_ppda</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="1" t="inlineStr">
         <is>
-          <t>home_total_assists</t>
+          <t>home_fouls</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
@@ -633,67 +633,67 @@
     <row r="18">
       <c r="A18" s="1" t="inlineStr">
         <is>
-          <t>home_total_xAssists</t>
+          <t>home_corners</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>home_total_key_passes</t>
+          <t>home_yellowCards</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>home_total_xGoalsChain</t>
+          <t>home_redCards</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="1" t="inlineStr">
         <is>
-          <t>home_total_xGoalsBuildup</t>
+          <t>home_total_assists</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="1" t="inlineStr">
         <is>
-          <t>home_total_yellow_cards</t>
+          <t>home_total_xAssists</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="1" t="inlineStr">
         <is>
-          <t>home_total_red_cards</t>
+          <t>home_total_key_passes</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
@@ -705,7 +705,7 @@
     <row r="24">
       <c r="A24" s="1" t="inlineStr">
         <is>
-          <t>home_total_blocked_shots</t>
+          <t>home_total_xGoalsChain</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
@@ -717,7 +717,7 @@
     <row r="25">
       <c r="A25" s="1" t="inlineStr">
         <is>
-          <t>home_total_saved_shots</t>
+          <t>home_total_xGoalsBuildup</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
@@ -729,19 +729,19 @@
     <row r="26">
       <c r="A26" s="1" t="inlineStr">
         <is>
-          <t>away_xGoals</t>
+          <t>home_total_yellow_cards</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" s="1" t="inlineStr">
         <is>
-          <t>away_shots</t>
+          <t>home_total_red_cards</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
@@ -753,31 +753,31 @@
     <row r="28">
       <c r="A28" s="1" t="inlineStr">
         <is>
-          <t>away_shotsOnTarget</t>
+          <t>home_total_blocked_shots</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" s="1" t="inlineStr">
         <is>
-          <t>away_deep</t>
+          <t>home_total_saved_shots</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="1" t="inlineStr">
         <is>
-          <t>away_ppda</t>
+          <t>away_xGoals</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
@@ -789,7 +789,7 @@
     <row r="31">
       <c r="A31" s="1" t="inlineStr">
         <is>
-          <t>away_fouls</t>
+          <t>away_shots</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
@@ -801,7 +801,7 @@
     <row r="32">
       <c r="A32" s="1" t="inlineStr">
         <is>
-          <t>away_corners</t>
+          <t>away_shotsOnTarget</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
@@ -813,31 +813,31 @@
     <row r="33">
       <c r="A33" s="1" t="inlineStr">
         <is>
-          <t>away_yellowCards</t>
+          <t>away_deep</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" s="1" t="inlineStr">
         <is>
-          <t>away_redCards</t>
+          <t>away_ppda</t>
         </is>
       </c>
       <c r="B34" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" s="1" t="inlineStr">
         <is>
-          <t>away_total_assists</t>
+          <t>away_fouls</t>
         </is>
       </c>
       <c r="B35" t="inlineStr">
@@ -849,67 +849,67 @@
     <row r="36">
       <c r="A36" s="1" t="inlineStr">
         <is>
-          <t>away_total_xAssists</t>
+          <t>away_corners</t>
         </is>
       </c>
       <c r="B36" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="1" t="inlineStr">
         <is>
-          <t>away_total_key_passes</t>
+          <t>away_yellowCards</t>
         </is>
       </c>
       <c r="B37" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" s="1" t="inlineStr">
         <is>
-          <t>away_total_xGoalsChain</t>
+          <t>away_redCards</t>
         </is>
       </c>
       <c r="B38" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" s="1" t="inlineStr">
         <is>
-          <t>away_total_xGoalsBuildup</t>
+          <t>away_total_assists</t>
         </is>
       </c>
       <c r="B39" t="inlineStr">
         <is>
-          <t>float64</t>
+          <t>int64</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" s="1" t="inlineStr">
         <is>
-          <t>away_total_yellow_cards</t>
+          <t>away_total_xAssists</t>
         </is>
       </c>
       <c r="B40" t="inlineStr">
         <is>
-          <t>int64</t>
+          <t>float64</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" s="1" t="inlineStr">
         <is>
-          <t>away_total_red_cards</t>
+          <t>away_total_key_passes</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
@@ -921,7 +921,7 @@
     <row r="42">
       <c r="A42" s="1" t="inlineStr">
         <is>
-          <t>away_total_blocked_shots</t>
+          <t>away_total_xGoalsChain</t>
         </is>
       </c>
       <c r="B42" t="inlineStr">
@@ -933,7 +933,7 @@
     <row r="43">
       <c r="A43" s="1" t="inlineStr">
         <is>
-          <t>away_total_saved_shots</t>
+          <t>away_total_xGoalsBuildup</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
@@ -945,10 +945,58 @@
     <row r="44">
       <c r="A44" s="1" t="inlineStr">
         <is>
+          <t>away_total_yellow_cards</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>int64</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" s="1" t="inlineStr">
+        <is>
+          <t>away_total_red_cards</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>int64</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" s="1" t="inlineStr">
+        <is>
+          <t>away_total_blocked_shots</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" s="1" t="inlineStr">
+        <is>
+          <t>away_total_saved_shots</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>float64</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" s="1" t="inlineStr">
+        <is>
           <t>gameresult</t>
         </is>
       </c>
-      <c r="B44" t="inlineStr">
+      <c r="B48" t="inlineStr">
         <is>
           <t>object</t>
         </is>

</xml_diff>